<commit_message>
adding test cae to verift sales data on SalesTargets page
</commit_message>
<xml_diff>
--- a/target/classes/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/target/classes/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F0C170-A1A0-4595-A044-ECB9DF854AE3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269F847E-CC16-4CC1-8DBB-3B290D9FCAFD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4320" windowWidth="20490" windowHeight="5535" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="calendar" sheetId="7" r:id="rId7"/>
     <sheet name="forms" sheetId="8" r:id="rId8"/>
     <sheet name="case" sheetId="9" r:id="rId9"/>
-    <sheet name="FacebookSignup" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="203">
   <si>
     <t>title</t>
   </si>
@@ -638,34 +637,13 @@
   </si>
   <si>
     <t>General Support</t>
-  </si>
-  <si>
-    <t>fName</t>
-  </si>
-  <si>
-    <t>lName</t>
-  </si>
-  <si>
-    <t>mobilrNum</t>
-  </si>
-  <si>
-    <t>newPassword</t>
-  </si>
-  <si>
-    <t>Tejas</t>
-  </si>
-  <si>
-    <t>Niturkar</t>
-  </si>
-  <si>
-    <t>TestPass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -677,14 +655,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -717,14 +687,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1154,53 +1123,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CD0068-5A10-4CC8-AFC0-8D2E22B0AAD0}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2">
-        <v>9489349484</v>
-      </c>
-      <c r="D2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309976B7-D42A-4B2F-AA38-58A2E3AB0FAF}">
   <dimension ref="A1:H2"/>
@@ -2047,7 +1969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C93E2B-3F3D-4064-BEA2-98FA9152DF33}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>